<commit_message>
Almost finished revamping the Fighter skill.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/SkillTemplate.xlsx
+++ b/GameDesign/Class/SkillTemplate.xlsx
@@ -13,6 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
+    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
+    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
+    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
+    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
+    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
+    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -50,9 +59,6 @@
     <t>[[Max effect accumulation: - ]]</t>
   </si>
   <si>
-    <t>[[Number of turns between two casts: - tours ]]</t>
-  </si>
-  <si>
     <t>[[Line of sight: - ]]</t>
   </si>
   <si>
@@ -75,6 +81,15 @@
   </si>
   <si>
     <t>SKILL NAME</t>
+  </si>
+  <si>
+    <t>Effect name: ''X''.</t>
+  </si>
+  <si>
+    <t>Unbuff ''X'' effect.</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: -  ]]</t>
   </si>
 </sst>
 </file>
@@ -161,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -181,6 +196,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,7 +517,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +537,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -531,14 +549,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -583,7 +601,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -602,7 +620,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -640,7 +658,7 @@
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -652,14 +670,14 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -677,7 +695,7 @@
     <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
       <c r="C29" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -688,12 +706,1969 @@
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="1"/>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started the Hunter skill documentation. 3/10 completed.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/SkillTemplate.xlsx
+++ b/GameDesign/Class/SkillTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>